<commit_message>
creation of "baseline" case
1. imported key defaults from bioluc scenarios 2020-08-04.xlsx
2. Checked compared model with earlier version to ensure consistency in input data
3. enhanced outputs table so that now have key indicators for all regions
4. created tables for commodity products (maize, wheat, oilcrop) and animal products imports. Format is Product, to country, from country.
5. set up data links for product, to country, from country tables to csv files.
6. moved old and unused spreadsheets to "old and unused data" folder.
</commit_message>
<xml_diff>
--- a/Models/BioLUC-CRAFTY-2000/Data/BioLUCScenarios.xlsx
+++ b/Models/BioLUC-CRAFTY-2000/Data/BioLUCScenarios.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\GitHub\CRAFTY-BioLuc\Models\BioLUC-CRAFTY-2000\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\millington\2020-08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19231C6F-0339-4980-8F77-6B489337A91F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A340E87-A02E-4D01-A201-73939F9E8127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29610" yWindow="1395" windowWidth="24765" windowHeight="13485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ToStella" sheetId="1" r:id="rId1"/>
+    <sheet name="Baseline" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
     <author>Steve Peterson</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{D65BF5D5-B715-4788-A298-839CD9F2D1AB}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{7C56FB9F-B0A0-4165-ADF3-E3B1B2EDECCD}">
       <text>
         <r>
           <rPr>
@@ -44,7 +45,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -53,14 +54,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Set this to 1 to activate connection from BioLUC to CRAFTY. Set to 0 to run Bioluc Brazil module</t>
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{FD3205E7-37B0-4DF6-87C0-15E0EC3B2152}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{33A4DF32-34F3-4479-BD1F-F999FBCFA789}">
       <text>
         <r>
           <rPr>
@@ -68,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -77,14 +78,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 index of responsiveness in Brazil to global shortfall of Maize.  Higher values incicate higher responiveness within Brazil</t>
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6C56AC94-91E1-41C1-B851-09A937BBD0A6}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{DAB975EE-2B2E-49B2-800A-6D9786B8748F}">
       <text>
         <r>
           <rPr>
@@ -92,7 +93,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -101,14 +102,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 index of responsiveness in Brazil to global shortfall of Soy  Higher values incicate higher responiveness within Brazil</t>
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{27C10743-7379-4D19-984C-D705B036C906}">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{632ADA47-DEE5-4611-826F-A0B4D031A0F0}">
       <text>
         <r>
           <rPr>
@@ -116,7 +117,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -125,14 +126,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 index of responsiveness in Brazil to global shortfall of Beef.  Higher values incicate higher responiveness within Brazil</t>
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{AA65400F-9D22-4DA5-85F4-6FEA78B9D7B5}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{39693C46-9C44-47E9-ADA9-B871F39A3C11}">
       <text>
         <r>
           <rPr>
@@ -140,7 +141,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -149,14 +150,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 % deviation from yield trend, by year</t>
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{38287FC8-6546-4198-82E6-4687A246B239}">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{D7449C21-B7AE-4906-858B-B9CD4A0E980E}">
       <text>
         <r>
           <rPr>
@@ -164,7 +165,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -173,14 +174,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 % deviation from yield trend, by year</t>
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{4542282E-8AA9-4C22-B20E-7AA0DA7457BC}">
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{6A61AEB8-3AD4-49C6-AA59-EE093BFD7AE6}">
       <text>
         <r>
           <rPr>
@@ -188,7 +189,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -197,14 +198,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 % deviation from yield trend, by year</t>
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{0C9BCED2-ED43-4FEB-93F2-E85C207A3E5D}">
+    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{15E21A1A-E8FC-427F-875B-6E69EB7B45A6}">
       <text>
         <r>
           <rPr>
@@ -212,7 +213,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -221,14 +222,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 % deviation from yield trend, by year</t>
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{1B559E70-A35C-485C-B9F1-77924EBCC053}">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{6293E722-FD13-4773-B655-DCD73F02CD93}">
       <text>
         <r>
           <rPr>
@@ -248,11 +249,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-test note</t>
+(beef/dairy/pork/chicken) Switch for China diet transition
+Set to fractional value to capture portion of gap between traditional and western diet that is realized over ~3 transition times</t>
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{704652FD-46A9-4492-B794-D1DA791BF043}">
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{E3C68243-16A5-4A28-A1FB-5CC94F732B72}">
       <text>
         <r>
           <rPr>
@@ -260,7 +262,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -269,14 +271,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-time to begin transition in China toward Western Diet </t>
+default was 0.  Set to 0.5 to increase beef portion of diet to 50% of western value</t>
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{1B5FA1A1-F9AD-4762-9537-D2DA1FC4C0F1}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{06B50403-146B-444E-AFDC-185AC2EEEB0D}">
       <text>
         <r>
           <rPr>
@@ -284,7 +286,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Peterson:</t>
         </r>
@@ -293,14 +295,41 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-exponential averaging time for making transition from china diet trend to western diet trajectory</t>
+time to begin transition in China toward Western Diet 
+Default is 2020.
+Set to 2010 to initiate movement from traditional to western diet in 2010</t>
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{2E9166B3-99C0-40B3-B7C6-645EF2C62965}">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{12CCE4D4-E876-43E4-A1AB-796935001AC5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+exponential averaging time for making transition from china diet trend to western diet trajectory
+95% of gap between US and China is eliminated in ~3x transition times.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{F0F4418F-4437-4D83-8F72-D9E956BB8984}">
       <text>
         <r>
           <rPr>
@@ -324,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{F1A64087-0769-4A65-8EB4-8274B1F0FE12}">
+    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{212176CE-97C4-4599-9139-5DB42F329393}">
       <text>
         <r>
           <rPr>
@@ -348,7 +377,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{FB008054-18EE-4175-B037-ADF6115AAF21}">
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{9F317545-BD7C-4CA7-9DC7-4E6887B8D90A}">
       <text>
         <r>
           <rPr>
@@ -372,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{C5AC1108-3C90-4F9E-893B-7A5079D9E6D5}">
+    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{A27D3B8A-CE42-44E0-AF4E-1B879916CE7F}">
       <text>
         <r>
           <rPr>
@@ -401,7 +430,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Global.BRA_Maize_Responsiveness</t>
   </si>
@@ -455,26 +484,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -497,8 +513,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +546,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -536,11 +565,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,19 +852,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2001</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2002</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2003</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2004</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2005</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2006</v>
+      </c>
+      <c r="H1" s="3">
+        <v>2007</v>
+      </c>
+      <c r="I1" s="3">
+        <v>2008</v>
+      </c>
+      <c r="J1" s="3">
+        <v>2009</v>
+      </c>
+      <c r="K1" s="3">
+        <v>2010</v>
+      </c>
+      <c r="L1" s="3">
+        <v>2011</v>
+      </c>
+      <c r="M1" s="3">
+        <v>2012</v>
+      </c>
+      <c r="N1" s="3">
+        <v>2013</v>
+      </c>
+      <c r="O1" s="3">
+        <v>2014</v>
+      </c>
+      <c r="P1" s="3">
+        <v>2015</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="R1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="S1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="T1" s="3">
+        <v>2019</v>
+      </c>
+      <c r="U1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="V1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="W1" s="3">
+        <v>2022</v>
+      </c>
+      <c r="X1" s="3">
+        <v>2023</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>2024</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>2025</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>2026</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>2027</v>
+      </c>
+      <c r="AC1" s="3">
+        <v>2028</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>2029</v>
+      </c>
+      <c r="AE1" s="3">
+        <v>2030</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D9F6D-FD33-4AB2-9981-3A5DBF23E69E}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.26171875" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -927,15 +1073,15 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1030,102 +1176,102 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>0.60899999999999999</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="R7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="S7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="W7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="X7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Z7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AA7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AB7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AC7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AD7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AE7">
-        <v>0.60899999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1220,7 +1366,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1315,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1410,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1505,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1600,32 +1746,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
+      <c r="B19" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B21">
-        <v>2020</v>
+      <c r="B21" s="6">
+        <v>2010</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1633,7 +1781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1641,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1649,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1657,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
creates additional scenarios for mashup work
additional sheets in scenarios spreadsheet to capture demand, yield variations.
Modifications to model to accept new scenarios.
</commit_message>
<xml_diff>
--- a/Models/BioLUC-CRAFTY-2000/Data/BioLUCScenarios.xlsx
+++ b/Models/BioLUC-CRAFTY-2000/Data/BioLUCScenarios.xlsx
@@ -5,16 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\millington\2020-08\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\GitHub\CRAFTY-BioLuc\Models\BioLUC-CRAFTY-2000\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A340E87-A02E-4D01-A201-73939F9E8127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D89A08-A575-41A5-B9EC-ADAB36A32D4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="1395" windowWidth="24765" windowHeight="13485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="690" windowWidth="24765" windowHeight="14910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ToStella" sheetId="1" r:id="rId1"/>
     <sheet name="Baseline" sheetId="2" r:id="rId2"/>
+    <sheet name="PermChangeAPImports" sheetId="3" r:id="rId3"/>
+    <sheet name="TempChangeAPImports" sheetId="4" r:id="rId4"/>
+    <sheet name="APDemandChg" sheetId="5" r:id="rId5"/>
+    <sheet name="CPYieldChg" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,6 +41,40 @@
     <author>Steve Peterson</author>
   </authors>
   <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{05591E52-D1A5-40F7-B567-209D21CF95E3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Set this to 1 to activate connection from BioLUC to CRAFTY. Set to 0 to run Bioluc Brazil module</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Steve Peterson</author>
+  </authors>
+  <commentList>
     <comment ref="A3" authorId="0" shapeId="0" xr:uid="{7C56FB9F-B0A0-4165-ADF3-E3B1B2EDECCD}">
       <text>
         <r>
@@ -329,7 +367,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{F0F4418F-4437-4D83-8F72-D9E956BB8984}">
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{3B803102-BA94-480B-8F78-4D1D538858EF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphical function that sets ramp in of AP demand change
+Set ramp-in ranges from 0 to 1 over period 2020-2030</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{F0F4418F-4437-4D83-8F72-D9E956BB8984}">
       <text>
         <r>
           <rPr>
@@ -353,7 +416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{212176CE-97C4-4599-9139-5DB42F329393}">
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{212176CE-97C4-4599-9139-5DB42F329393}">
       <text>
         <r>
           <rPr>
@@ -377,7 +440,80 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{9F317545-BD7C-4CA7-9DC7-4E6887B8D90A}">
+    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{46412E2D-57D6-412B-9B98-78A095F73D1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphical function that sets ramp in CP yield change
+set to 1 for year(s) in which yield change is active over 2020-2030. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{9C21B993-6F02-4BB3-9D8B-1B256919781C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline yield trajectory for commodity products in this region</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{A9BCC558-64CC-4109-A52F-2DC95A80453E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline yield trajectory for commodity products in this region</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A37" authorId="0" shapeId="0" xr:uid="{5C185038-81F8-4987-843C-C63EFD63AAB3}">
       <text>
         <r>
           <rPr>
@@ -401,27 +537,601 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{A27D3B8A-CE42-44E0-AF4E-1B879916CE7F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Steve Peterson:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction of animal product (beef/dairy/pork/chicken) that is imported vs produced domestically</t>
+    <comment ref="A39" authorId="0" shapeId="0" xr:uid="{9F317545-BD7C-4CA7-9DC7-4E6887B8D90A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline diet trajectory for animal products</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{A27D3B8A-CE42-44E0-AF4E-1B879916CE7F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction of animal product (beef/dairy/pork/chicken) potential import demand that is desired to be imported vs produced domestically
+2020-08-06. old values are 0.2/0/0.02/0.1  Changed in model to
+0.3/0/0.5/0.1 in context of implementing Jem scenarios</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{CB2E4E1B-AC4B-4794-B526-30FFC61CA10B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+switch to activate change in import profile for China. 1 means active. 0 means default values for BaseAPImportFraction</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Steve Peterson</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{85841668-3542-4456-B367-8D2B53A5C639}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Set this to 1 to activate connection from BioLUC to CRAFTY. Set to 0 to run Bioluc Brazil module</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{15C1735F-8F68-4F21-990B-20C59FFB4EED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+switch to activate change in import profile for China. 1 means active. 0 means default values for BaseAPImportFraction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{66126331-5C7F-4DB2-86B7-AB8F80AA4C6F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+start time for change in import profile for China. Default is 2017. Import switch must be set to 1 for scenario to take effect.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{326E22D0-926C-4F64-8EAD-3EC7B484D5A2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+start time for change in import profile for China. Value of 2050 holds scenario in place to end of simulation. Import switch must be set to 1 for scenario to take effect.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{DDA69CFB-002F-4834-AD99-444D6797867A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Additional fraction of animal product (beef/dairy/pork/chicken) import demand that is imported vs produced domestically
+Given default values for BaseAPImportFraction, values here should not be greater than 0.7/1/0.5/0.9</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Steve Peterson</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{AE2B8608-8F86-48C5-9A33-7AF9E2B3D5D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Set this to 1 to activate connection from BioLUC to CRAFTY. Set to 0 to run Bioluc Brazil module</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{2F60550E-8E69-4788-AD39-5A06C4FDB6B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+switch to activate change in import profile for China. 1 means active. 0 means default values for BaseAPImportFraction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{F0A3D2A7-0BF8-415B-B314-7692A90A7130}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+start time for change in import profile for China. Default is 2017. Import switch must be set to 1 for scenario to take effect.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{30E8604B-2128-47AD-A98A-3F22FB446A13}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+start time for change in import profile for China. Value of 2050 holds scenario in place to end of simulation. Import switch must be set to 1 for scenario to take effect.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{B22F2D01-75D8-4982-BF6F-DAF43ED36ADB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Additional fraction of animal product (beef/dairy/pork/chicken) import demand that is imported vs produced domestically
+Given default values for BaseAPImportFraction, values here should not be greater than 0.7/1/0.5/0.9</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Steve Peterson</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{753F6B85-B8A6-4F01-9C79-E9E7275E34CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Set this to 1 to activate connection from BioLUC to CRAFTY. Set to 0 to run Bioluc Brazil module</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{E392B96E-6D82-4736-BF91-D1672492B40E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphical function that sets ramp in of AP demand change
+Set ramp-in ranges from 0 to 1 over period 2020-2030</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{18784269-CCB0-4E82-940C-9A22F620E57F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline diet trajectory for animal products</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{4FCA4B3F-3235-442A-A87C-53F1A2535553}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline diet trajectory for animal products</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{021EBA60-E9CE-4F5D-BB76-EEF19051726B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline diet trajectory for animal products</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Steve Peterson</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{097CA6B6-EE25-458D-9C37-6F2FE344FF33}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Set this to 1 to activate connection from BioLUC to CRAFTY. Set to 0 to run Bioluc Brazil module</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{23D55E0A-2BAE-49AE-9368-6383D873010A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphical function that sets ramp in CP yield change
+set to 1 for year(s) in which yield change is active over 2020-2030. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{B1125820-8396-4F4D-A4B7-8F87ACEFC4B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline yield trajectory for commodity products in this region</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{52B932E0-D4F2-483E-8462-FBCF48F1B594}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline yield trajectory for commodity products in this region</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{45DD5214-C8BC-44DD-AE7D-CE489202C00D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Peterson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage deviation from baseline diet trajectory for animal products</t>
         </r>
       </text>
     </comment>
@@ -430,7 +1140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>Global.BRA_Maize_Responsiveness</t>
   </si>
@@ -477,7 +1187,34 @@
     <t>Global.Crafty active</t>
   </si>
   <si>
-    <t>CHIHKG.APImportFraction[AnimalProduct]</t>
+    <t>CHIHKG.ChangeAPImportSwitch</t>
+  </si>
+  <si>
+    <t>CHIHKG.ChangeAPImportStart</t>
+  </si>
+  <si>
+    <t>CHIHKG.ChangeAPImportStop</t>
+  </si>
+  <si>
+    <t>CHIHKG.BaseAPImportFraction[AnimalProduct]</t>
+  </si>
+  <si>
+    <t>CHIHKG.APImportFractionChgAMT[AnimalProduct]</t>
+  </si>
+  <si>
+    <t>Global.AP demand ramp in logic</t>
+  </si>
+  <si>
+    <t>Global.CP yield ramp in logic</t>
+  </si>
+  <si>
+    <t>Global.CP yield mod pct[USA 1]</t>
+  </si>
+  <si>
+    <t>Global.CP yield mod pct[EU27 1]</t>
+  </si>
+  <si>
+    <t>Global.CP yield mod pct[CHIHKG 1]</t>
   </si>
 </sst>
 </file>
@@ -852,11 +1589,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,18 +1696,27 @@
         <v>2030</v>
       </c>
     </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D9F6D-FD33-4AB2-9981-3A5DBF23E69E}">
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J38" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,23 +2529,54 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1807,19 +2584,97 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <v>0.3</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0.5</v>
+      </c>
+      <c r="E41">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>15</v>
       </c>
-      <c r="B31">
-        <v>0.2</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0.02</v>
-      </c>
-      <c r="E31">
-        <v>0.1</v>
+      <c r="B43">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1827,4 +2682,699 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2709315B-5C30-4B3C-9545-8F54E4310640}">
+  <dimension ref="A1:AE11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2001</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2002</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2003</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2004</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2005</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2006</v>
+      </c>
+      <c r="H1" s="3">
+        <v>2007</v>
+      </c>
+      <c r="I1" s="3">
+        <v>2008</v>
+      </c>
+      <c r="J1" s="3">
+        <v>2009</v>
+      </c>
+      <c r="K1" s="3">
+        <v>2010</v>
+      </c>
+      <c r="L1" s="3">
+        <v>2011</v>
+      </c>
+      <c r="M1" s="3">
+        <v>2012</v>
+      </c>
+      <c r="N1" s="3">
+        <v>2013</v>
+      </c>
+      <c r="O1" s="3">
+        <v>2014</v>
+      </c>
+      <c r="P1" s="3">
+        <v>2015</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="R1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="S1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="T1" s="3">
+        <v>2019</v>
+      </c>
+      <c r="U1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="V1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="W1" s="3">
+        <v>2022</v>
+      </c>
+      <c r="X1" s="3">
+        <v>2023</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>2024</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>2025</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>2026</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>2027</v>
+      </c>
+      <c r="AC1" s="3">
+        <v>2028</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>2029</v>
+      </c>
+      <c r="AE1" s="3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0.7</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F2B1A9-441C-4109-AD90-5F41692BEED0}">
+  <dimension ref="A1:AE10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2001</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2002</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2003</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2004</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2005</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2006</v>
+      </c>
+      <c r="H1" s="3">
+        <v>2007</v>
+      </c>
+      <c r="I1" s="3">
+        <v>2008</v>
+      </c>
+      <c r="J1" s="3">
+        <v>2009</v>
+      </c>
+      <c r="K1" s="3">
+        <v>2010</v>
+      </c>
+      <c r="L1" s="3">
+        <v>2011</v>
+      </c>
+      <c r="M1" s="3">
+        <v>2012</v>
+      </c>
+      <c r="N1" s="3">
+        <v>2013</v>
+      </c>
+      <c r="O1" s="3">
+        <v>2014</v>
+      </c>
+      <c r="P1" s="3">
+        <v>2015</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="R1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="S1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="T1" s="3">
+        <v>2019</v>
+      </c>
+      <c r="U1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="V1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="W1" s="3">
+        <v>2022</v>
+      </c>
+      <c r="X1" s="3">
+        <v>2023</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>2024</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>2025</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>2026</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>2027</v>
+      </c>
+      <c r="AC1" s="3">
+        <v>2028</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>2029</v>
+      </c>
+      <c r="AE1" s="3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>0.7</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E65D51-C03E-4665-A7FC-EF97F7DF7B4C}">
+  <dimension ref="A1:AE11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A5:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2001</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2002</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2003</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2004</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2005</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2006</v>
+      </c>
+      <c r="H1" s="3">
+        <v>2007</v>
+      </c>
+      <c r="I1" s="3">
+        <v>2008</v>
+      </c>
+      <c r="J1" s="3">
+        <v>2009</v>
+      </c>
+      <c r="K1" s="3">
+        <v>2010</v>
+      </c>
+      <c r="L1" s="3">
+        <v>2011</v>
+      </c>
+      <c r="M1" s="3">
+        <v>2012</v>
+      </c>
+      <c r="N1" s="3">
+        <v>2013</v>
+      </c>
+      <c r="O1" s="3">
+        <v>2014</v>
+      </c>
+      <c r="P1" s="3">
+        <v>2015</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="R1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="S1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="T1" s="3">
+        <v>2019</v>
+      </c>
+      <c r="U1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="V1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="W1" s="3">
+        <v>2022</v>
+      </c>
+      <c r="X1" s="3">
+        <v>2023</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>2024</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>2025</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>2026</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>2027</v>
+      </c>
+      <c r="AC1" s="3">
+        <v>2028</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>2029</v>
+      </c>
+      <c r="AE1" s="3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
+        <v>0.3</v>
+      </c>
+      <c r="F5">
+        <v>0.4</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>0.6</v>
+      </c>
+      <c r="I5">
+        <v>0.7</v>
+      </c>
+      <c r="J5">
+        <v>0.8</v>
+      </c>
+      <c r="K5">
+        <v>0.9</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>-20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0C4F16-A92E-424A-9A6E-F7F767AA8C5E}">
+  <dimension ref="A1:AE11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A5:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2001</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2002</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2003</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2004</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2005</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2006</v>
+      </c>
+      <c r="H1" s="3">
+        <v>2007</v>
+      </c>
+      <c r="I1" s="3">
+        <v>2008</v>
+      </c>
+      <c r="J1" s="3">
+        <v>2009</v>
+      </c>
+      <c r="K1" s="3">
+        <v>2010</v>
+      </c>
+      <c r="L1" s="3">
+        <v>2011</v>
+      </c>
+      <c r="M1" s="3">
+        <v>2012</v>
+      </c>
+      <c r="N1" s="3">
+        <v>2013</v>
+      </c>
+      <c r="O1" s="3">
+        <v>2014</v>
+      </c>
+      <c r="P1" s="3">
+        <v>2015</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="R1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="S1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="T1" s="3">
+        <v>2019</v>
+      </c>
+      <c r="U1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="V1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="W1" s="3">
+        <v>2022</v>
+      </c>
+      <c r="X1" s="3">
+        <v>2023</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>2024</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>2025</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>2026</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>2027</v>
+      </c>
+      <c r="AC1" s="3">
+        <v>2028</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>2029</v>
+      </c>
+      <c r="AE1" s="3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>